<commit_message>
Error file & xlsx update
</commit_message>
<xml_diff>
--- a/Team_DDGK_Report.xlsx
+++ b/Team_DDGK_Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krutarth\Desktop\cs555\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Stevens\CS 555\SSW-555-DDGK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D893B2-B3BB-43D4-A169-C8CE882D742E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2915F1A7-6294-4326-B83E-89BEEFD1ED1B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="219">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -179,15 +179,6 @@
     <t>GitHub Repository:</t>
   </si>
   <si>
-    <t>Bring pizza to our meetings</t>
-  </si>
-  <si>
-    <t>Leaving leftover pizza on the counter</t>
-  </si>
-  <si>
-    <t>Bring silverware for everyone</t>
-  </si>
-  <si>
     <t>Dates (birth, marriage, divorce, death) should not be after the current date</t>
   </si>
   <si>
@@ -720,6 +711,24 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Started</t>
+  </si>
+  <si>
+    <t>coming late for team meeting</t>
+  </si>
+  <si>
+    <t>missing deadline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">collborating with team </t>
+  </si>
+  <si>
+    <t>communication by slack</t>
+  </si>
+  <si>
+    <t>halping group members</t>
   </si>
 </sst>
 </file>
@@ -1000,7 +1009,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1077,6 +1086,10 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1329,7 +1342,7 @@
                   <c:v>42046</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42058</c:v>
+                  <c:v>42061</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2234,20 +2247,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="120" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.69140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.69140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.69140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.84375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2264,80 +2277,80 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="E3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B4" t="s">
         <v>190</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" t="s">
         <v>191</v>
       </c>
-      <c r="C3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D3" s="17" t="s">
+      <c r="D4" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="E4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B5" t="s">
         <v>195</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>190</v>
-      </c>
-      <c r="B4" t="s">
-        <v>193</v>
-      </c>
-      <c r="C4" t="s">
-        <v>194</v>
-      </c>
-      <c r="D4" s="17" t="s">
+      <c r="D5" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="E5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>187</v>
+      </c>
+      <c r="B6" t="s">
         <v>197</v>
       </c>
-      <c r="E4" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>189</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C6" t="s">
         <v>198</v>
       </c>
-      <c r="C5" t="s">
-        <v>199</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="E5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>190</v>
-      </c>
-      <c r="B6" t="s">
-        <v>200</v>
-      </c>
-      <c r="C6" t="s">
-        <v>201</v>
-      </c>
       <c r="D6" s="17" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E6" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -2362,15 +2375,15 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView zoomScale="87" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:D17"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.3046875" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="18.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="4" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -2387,554 +2400,554 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3</v>
       </c>
       <c r="B18" s="35" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C18" s="35" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3</v>
       </c>
       <c r="B19" s="35" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C19" s="35" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E19" s="30" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E20" s="30" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E22" s="30" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E23" s="30" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>4</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>4</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>4</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>4</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>4</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>4</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>4</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>4</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D33" s="24" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E34" s="30"/>
     </row>
-    <row r="35" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E35" s="30"/>
     </row>
   </sheetData>
@@ -2948,53 +2961,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.84375" style="2"/>
-    <col min="2" max="2" width="9.4609375" customWidth="1"/>
-    <col min="3" max="3" width="15.84375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.3046875" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="2"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.25" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>159</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>162</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>0</v>
@@ -3015,9 +3028,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B15" s="11">
         <v>42046</v>
@@ -3031,9 +3044,9 @@
       <c r="F15" s="12"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B16" s="11">
         <v>42059</v>
@@ -3056,9 +3069,9 @@
         <v>87.5</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B17" s="11">
         <v>42071</v>
@@ -3071,7 +3084,7 @@
         <v>8</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F17" s="13">
         <f>-H20</f>
@@ -3082,9 +3095,9 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B18" s="11">
         <v>42091</v>
@@ -3097,7 +3110,7 @@
         <v>8</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F18" s="13">
         <v>0</v>
@@ -3107,9 +3120,9 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B19" s="11">
         <v>42108</v>
@@ -3122,7 +3135,7 @@
         <v>8</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F19" s="13">
         <v>0</v>
@@ -3141,33 +3154,33 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:Q21"/>
+  <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView zoomScale="66" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.69140625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.75" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.15234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.84375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.4609375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.69140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.4609375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.3046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.4609375" style="15" customWidth="1"/>
+    <col min="4" max="4" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.5" style="15" customWidth="1"/>
     <col min="12" max="12" width="25" style="15" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.69140625" style="15"/>
-    <col min="15" max="15" width="9.15234375" style="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.75" style="15"/>
+    <col min="15" max="15" width="9.125" style="15" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14" style="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.15234375" style="15" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.125" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3193,39 +3206,39 @@
         <v>16</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="K1" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="L1" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="M1" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="P1" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q1" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="M1" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="O1" s="14" t="s">
-        <v>181</v>
-      </c>
-      <c r="P1" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q1" s="14" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E2">
         <v>15</v>
@@ -3233,35 +3246,38 @@
       <c r="F2">
         <v>30</v>
       </c>
+      <c r="G2">
+        <v>8</v>
+      </c>
       <c r="H2">
         <v>35</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M2" s="16"/>
       <c r="O2" s="16"/>
       <c r="P2" s="16"/>
       <c r="Q2" s="16"/>
     </row>
-    <row r="3" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B3" s="41" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E3">
         <v>20</v>
@@ -3269,31 +3285,34 @@
       <c r="F3">
         <v>45</v>
       </c>
+      <c r="G3">
+        <v>28</v>
+      </c>
       <c r="H3">
         <v>25</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="K3" s="16" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B4" s="41" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E4">
         <v>20</v>
@@ -3301,31 +3320,34 @@
       <c r="F4">
         <v>30</v>
       </c>
+      <c r="G4">
+        <v>14</v>
+      </c>
       <c r="H4">
         <v>45</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="K4" s="16" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="41" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B5" s="41" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E5">
         <v>25</v>
@@ -3333,31 +3355,34 @@
       <c r="F5">
         <v>45</v>
       </c>
+      <c r="G5">
+        <v>14</v>
+      </c>
       <c r="H5">
         <v>25</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="K5" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="L5" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="L5" s="16" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="41" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B6" s="41" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E6">
         <v>25</v>
@@ -3365,31 +3390,34 @@
       <c r="F6">
         <v>30</v>
       </c>
+      <c r="G6">
+        <v>32</v>
+      </c>
       <c r="H6">
         <v>30</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="41" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B7" s="41" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E7">
         <v>25</v>
@@ -3397,31 +3425,34 @@
       <c r="F7">
         <v>25</v>
       </c>
+      <c r="G7">
+        <v>40</v>
+      </c>
       <c r="H7">
         <v>30</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="41" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E8">
         <v>30</v>
@@ -3429,35 +3460,38 @@
       <c r="F8">
         <v>20</v>
       </c>
+      <c r="G8">
+        <v>22</v>
+      </c>
       <c r="H8">
         <v>30</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="M8" s="16"/>
       <c r="O8" s="16"/>
       <c r="P8" s="16"/>
       <c r="Q8" s="16"/>
     </row>
-    <row r="9" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="41" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B9" s="41" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E9">
         <v>25</v>
@@ -3465,53 +3499,70 @@
       <c r="F9">
         <v>60</v>
       </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
       <c r="H9">
         <v>45</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="L9" s="16" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D10" s="30"/>
-    </row>
-    <row r="14" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <f>SUM(G2:G9)</f>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="5"/>
     </row>
-    <row r="16" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="42" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="42" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="42" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="1" t="s">
-        <v>36</v>
+    <row r="21" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="42" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="42" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -3525,21 +3576,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A2" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.84375" style="2"/>
-    <col min="2" max="2" width="16.69140625" customWidth="1"/>
-    <col min="3" max="3" width="12.4609375" customWidth="1"/>
-    <col min="4" max="4" width="7.15234375" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="2"/>
+    <col min="2" max="2" width="16.75" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="7.125" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3559,20 +3610,29 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>42046</v>
       </c>
       <c r="B2">
         <v>32</v>
       </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
       <c r="D2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>42058</v>
+        <v>42061</v>
       </c>
       <c r="B3">
         <v>24</v>
@@ -3582,14 +3642,14 @@
         <v>8</v>
       </c>
       <c r="D3">
-        <v>350</v>
+        <v>165</v>
       </c>
       <c r="E3">
         <v>220</v>
       </c>
       <c r="F3" s="7">
         <f>(D3-D2)/E3*60</f>
-        <v>95.454545454545453</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -3604,16 +3664,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView zoomScale="73" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="2" max="2" width="25.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3642,18 +3702,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>200</v>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>197</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="E2">
         <v>15</v>
@@ -3662,18 +3722,18 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="32" t="s">
-        <v>124</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>193</v>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>190</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="E3">
         <v>20</v>
@@ -3682,18 +3742,18 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="32" t="s">
-        <v>125</v>
-      </c>
-      <c r="B4" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>193</v>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="43" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>190</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="E4">
         <v>20</v>
@@ -3702,18 +3762,18 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="26" t="s">
-        <v>126</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>198</v>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>195</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="E5">
         <v>25</v>
@@ -3722,18 +3782,18 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
-        <v>127</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>198</v>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>195</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="E6">
         <v>25</v>
@@ -3742,18 +3802,18 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>171</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>191</v>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>188</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="E7">
         <v>25</v>
@@ -3762,18 +3822,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>191</v>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>188</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="E8">
         <v>30</v>
@@ -3782,18 +3842,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>200</v>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>197</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="E9">
         <v>25</v>
@@ -3817,9 +3877,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3858,503 +3918,503 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="67" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B33"/>
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.4609375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E2" s="29"/>
       <c r="F2" s="30" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E3" s="28"/>
       <c r="F3" s="30" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E4" s="31"/>
       <c r="F4" s="30" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E5" s="34"/>
       <c r="F5" s="30" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="B6" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" s="27" t="s">
+      <c r="B9" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A12" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="A13" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="63" x14ac:dyDescent="0.2">
+      <c r="A14" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="C15" s="25" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.3">
-      <c r="A7" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" s="25" t="s">
+    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="25" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.3">
-      <c r="A8" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="C9" s="19" t="s">
+    <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="36" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="B18" s="35" t="s">
+        <v>175</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="B19" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="B20" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="38" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="B21" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="38" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A22" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A23" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A24" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="A25" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A26" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="B26" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" s="38" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="126" x14ac:dyDescent="0.2">
+      <c r="A27" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="B27" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" s="38" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.3">
-      <c r="A11" s="32" t="s">
-        <v>124</v>
-      </c>
-      <c r="B11" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="C11" s="33" t="s">
+    <row r="28" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A28" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A29" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="19" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.3">
-      <c r="A12" s="32" t="s">
-        <v>125</v>
-      </c>
-      <c r="B12" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="C12" s="33" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.3">
-      <c r="A13" s="26" t="s">
-        <v>126</v>
-      </c>
-      <c r="B13" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="C13" s="27" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.3">
-      <c r="A14" s="26" t="s">
-        <v>127</v>
-      </c>
-      <c r="B14" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="C14" s="27" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.3">
-      <c r="A15" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="B15" s="24" t="s">
-        <v>171</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.3">
-      <c r="A16" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="B16" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A17" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="B17" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="C17" s="25" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A18" s="35" t="s">
-        <v>131</v>
-      </c>
-      <c r="B18" s="35" t="s">
-        <v>178</v>
-      </c>
-      <c r="C18" s="36" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A19" s="35" t="s">
-        <v>132</v>
-      </c>
-      <c r="B19" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="C19" s="36" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A20" s="37" t="s">
-        <v>133</v>
-      </c>
-      <c r="B20" s="37" t="s">
-        <v>87</v>
-      </c>
-      <c r="C20" s="38" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A21" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="B21" s="37" t="s">
-        <v>88</v>
-      </c>
-      <c r="C21" s="38" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A22" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="B22" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="C22" s="25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A23" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="B23" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="C23" s="25" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A24" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.3">
-      <c r="A25" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="C25" s="19" t="s">
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="B30" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" s="40" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A26" s="37" t="s">
-        <v>139</v>
-      </c>
-      <c r="B26" s="37" t="s">
-        <v>95</v>
-      </c>
-      <c r="C26" s="38" t="s">
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="B31" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" s="40" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.3">
-      <c r="A27" s="37" t="s">
-        <v>140</v>
-      </c>
-      <c r="B27" s="37" t="s">
-        <v>96</v>
-      </c>
-      <c r="C27" s="38" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A28" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="B28" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="C28" s="19" t="s">
+    <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A32" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="B32" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="C32" s="23" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A29" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="B29" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="C29" s="19" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A30" s="39" t="s">
+    <row r="33" spans="1:3" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="B30" s="39" t="s">
+      <c r="B33" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="C30" s="40" t="s">
+      <c r="C33" s="23" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A31" s="39" t="s">
+    <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>144</v>
       </c>
-      <c r="B31" s="39" t="s">
+      <c r="B34" t="s">
         <v>100</v>
       </c>
-      <c r="C31" s="40" t="s">
+      <c r="C34" s="10" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A32" s="22" t="s">
+    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>145</v>
       </c>
-      <c r="B32" s="22" t="s">
+      <c r="B35" t="s">
+        <v>110</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>146</v>
+      </c>
+      <c r="B36" t="s">
         <v>101</v>
       </c>
-      <c r="C32" s="23" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="B33" s="22" t="s">
+      <c r="C36" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>147</v>
+      </c>
+      <c r="B37" t="s">
         <v>102</v>
       </c>
-      <c r="C33" s="23" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>147</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="C37" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>148</v>
+      </c>
+      <c r="B38" t="s">
         <v>103</v>
       </c>
-      <c r="C34" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>148</v>
-      </c>
-      <c r="B35" t="s">
-        <v>113</v>
-      </c>
-      <c r="C35" s="10" t="s">
+      <c r="C38" s="10" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="39" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>149</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B39" t="s">
         <v>104</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C39" s="10" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>150</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B40" t="s">
         <v>105</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C40" s="10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>151</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B41" t="s">
         <v>106</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C41" s="10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>152</v>
+      </c>
+      <c r="B42" t="s">
+        <v>108</v>
+      </c>
+      <c r="C42" s="10" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>152</v>
-      </c>
-      <c r="B39" t="s">
-        <v>107</v>
-      </c>
-      <c r="C39" s="10" t="s">
+    <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>153</v>
+      </c>
+      <c r="B43" t="s">
+        <v>109</v>
+      </c>
+      <c r="C43" s="10" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>153</v>
-      </c>
-      <c r="B40" t="s">
-        <v>108</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>154</v>
-      </c>
-      <c r="B41" t="s">
-        <v>109</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>155</v>
-      </c>
-      <c r="B42" t="s">
-        <v>111</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>156</v>
-      </c>
-      <c r="B43" t="s">
-        <v>112</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -4371,9 +4431,9 @@
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>

</xml_diff>